<commit_message>
add flow sort email
</commit_message>
<xml_diff>
--- a/CustomerList.xlsx
+++ b/CustomerList.xlsx
@@ -53,136 +53,16 @@
     <x:t>Rank</x:t>
   </x:si>
   <x:si>
-    <x:t>b@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trần Thị B</x:t>
+    <x:t>trangvth22411@st.uel.edu.vn</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Võ Thị Huyền Trang</x:t>
   </x:si>
   <x:si>
     <x:t>08/2025-09/2025</x:t>
   </x:si>
   <x:si>
     <x:t>Bronze</x:t>
-  </x:si>
-  <x:si>
-    <x:t>c@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Lê Minh C</x:t>
-  </x:si>
-  <x:si>
-    <x:t>d@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Phạm Thị D</x:t>
-  </x:si>
-  <x:si>
-    <x:t>e@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hoàng Văn E</x:t>
-  </x:si>
-  <x:si>
-    <x:t>khoatrinhtiendat@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Trịnh Tiến Đạt Khoa</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Diamond</x:t>
-  </x:si>
-  <x:si>
-    <x:t>candicesanders@yahoo.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>John Wyatt</x:t>
-  </x:si>
-  <x:si>
-    <x:t>gwalker@smith.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Theresa Mendez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>davidmckee@lee.info</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Jessica Fernandez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>robert28@yahoo.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kathryn Gordon</x:t>
-  </x:si>
-  <x:si>
-    <x:t>trangvth22411@st.uel.edu.vn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Võ Thị Huyền Trang</x:t>
-  </x:si>
-  <x:si>
-    <x:t>thomasjamie@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kelly Webster</x:t>
-  </x:si>
-  <x:si>
-    <x:t>mgonzalez@james-hawkins.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>James Gonzalez</x:t>
-  </x:si>
-  <x:si>
-    <x:t>briana42@hotmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>John Palmer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Silver</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bridgetwilson@yahoo.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Casey Archer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lannqh22411@st.uel.edu.vn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Stephen Smith</x:t>
-  </x:si>
-  <x:si>
-    <x:t>robinsimpson@conner-miller.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Steven Chandler</x:t>
-  </x:si>
-  <x:si>
-    <x:t>hieuntm22411@st.uel.edu.vn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Daniel Proctor</x:t>
-  </x:si>
-  <x:si>
-    <x:t>amy68@weeks.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Brittany Reed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lisamiller@mckinney.biz</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Craig Horn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>khainq224117@st.uel.edu.vn</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Nguyễn Quốc Khải</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -587,7 +467,7 @@
   <x:dimension ref="A1:E3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:E63"/>
+      <x:selection activeCell="A2" sqref="A2 A2:E21"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +503,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C2" s="0">
-        <x:v>1000000</x:v>
+        <x:v>2020000</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
         <x:v>12</x:v>
@@ -634,13 +514,13 @@
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <x:c r="A3" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="0">
-        <x:v>200000</x:v>
+        <x:v>2020000</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>12</x:v>
@@ -651,13 +531,13 @@
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="0">
-        <x:v>2000000</x:v>
+        <x:v>2020000</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
         <x:v>12</x:v>
@@ -668,13 +548,13 @@
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C5" s="0">
-        <x:v>300000</x:v>
+        <x:v>2020000</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>12</x:v>
@@ -685,273 +565,18 @@
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C6" s="0">
-        <x:v>11420000</x:v>
+        <x:v>2020000</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="A7" s="0" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C7" s="0">
-        <x:v>640000</x:v>
-      </x:c>
-      <x:c r="D7" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E7" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:5">
-      <x:c r="A8" s="0" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C8" s="0">
-        <x:v>720000</x:v>
-      </x:c>
-      <x:c r="D8" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E8" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
-      <x:c r="A9" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C9" s="0">
-        <x:v>720000</x:v>
-      </x:c>
-      <x:c r="D9" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E9" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
-      <x:c r="A10" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="C10" s="0">
-        <x:v>1050000</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
-        <x:v>31</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="C11" s="0">
-        <x:v>2340000</x:v>
-      </x:c>
-      <x:c r="D11" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E11" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="C12" s="0">
-        <x:v>2500000</x:v>
-      </x:c>
-      <x:c r="D12" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="A13" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="C13" s="0">
-        <x:v>2000000</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C14" s="0">
-        <x:v>3500000</x:v>
-      </x:c>
-      <x:c r="D14" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E14" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
-      <x:c r="A15" s="0" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C15" s="0">
-        <x:v>240000</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:5">
-      <x:c r="A16" s="0" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="C16" s="0">
-        <x:v>800000</x:v>
-      </x:c>
-      <x:c r="D16" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E16" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:5">
-      <x:c r="A17" s="0" t="s">
-        <x:v>44</x:v>
-      </x:c>
-      <x:c r="B17" s="0" t="s">
-        <x:v>45</x:v>
-      </x:c>
-      <x:c r="C17" s="0">
-        <x:v>1200000</x:v>
-      </x:c>
-      <x:c r="D17" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E17" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:5">
-      <x:c r="A18" s="0" t="s">
-        <x:v>46</x:v>
-      </x:c>
-      <x:c r="B18" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C18" s="0">
-        <x:v>720000</x:v>
-      </x:c>
-      <x:c r="D18" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E18" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:5">
-      <x:c r="A19" s="0" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="C19" s="0">
-        <x:v>1620000</x:v>
-      </x:c>
-      <x:c r="D19" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E19" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:5">
-      <x:c r="A20" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="C20" s="0">
-        <x:v>2500000</x:v>
-      </x:c>
-      <x:c r="D20" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="21" spans="1:5">
-      <x:c r="A21" s="0" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B21" s="0" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="C21" s="0">
-        <x:v>1050000</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E21" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>

</xml_diff>